<commit_message>
fix failing integration test
</commit_message>
<xml_diff>
--- a/testdata/invalid-testdata/excel2json/properties-invalid-object.xlsx
+++ b/testdata/invalid-testdata/excel2json/properties-invalid-object.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -89,24 +89,6 @@
   </si>
   <si>
     <t>Geonames</t>
-  </si>
-  <si>
-    <t>hasInterval</t>
-  </si>
-  <si>
-    <t>Time interval</t>
-  </si>
-  <si>
-    <t>Zeitintervall</t>
-  </si>
-  <si>
-    <t>hasSequenceBounds</t>
-  </si>
-  <si>
-    <t>IntervalValue</t>
-  </si>
-  <si>
-    <t>Interval</t>
   </si>
   <si>
     <t xml:space="preserve">  </t>
@@ -117,7 +99,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +141,12 @@
       <name val="Calibri (Textkörper)"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -207,7 +195,7 @@
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -518,7 +506,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
       <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
@@ -657,58 +645,25 @@
       <c r="O3" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="6"/>
+      <c r="B4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
-      <c r="G4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>27</v>
-      </c>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-      <c r="J4" s="7"/>
+      <c r="J4" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="K4" s="6"/>
-      <c r="L4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O4" s="4"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="6"/>
-      <c r="B5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>